<commit_message>
Spent too much on a Horchata man
</commit_message>
<xml_diff>
--- a/Budget Plan.xlsx
+++ b/Budget Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toolupcom-my.sharepoint.com/personal/solomon_manamel_pcstools_com/Documents/Desktop/Personal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="96" documentId="13_ncr:1_{4B516CEF-07BC-46FE-AFFB-163B992373ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{71C068F1-2FCE-48B8-83BC-E83C6B6D7A69}"/>
+  <xr:revisionPtr revIDLastSave="148" documentId="13_ncr:1_{4B516CEF-07BC-46FE-AFFB-163B992373ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8D4B00DF-C374-4FBE-B51C-57A8DFCF4BDA}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="1635" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Add-ons" sheetId="7" r:id="rId1"/>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="190">
   <si>
     <t>To be allocated:</t>
   </si>
@@ -662,6 +662,27 @@
   </si>
   <si>
     <t>Tinder Messages 3</t>
+  </si>
+  <si>
+    <t>Bagel Nook</t>
+  </si>
+  <si>
+    <t>Taco Bell</t>
+  </si>
+  <si>
+    <t>SafeNest </t>
+  </si>
+  <si>
+    <t>Meow Wolf's Omega Mart</t>
+  </si>
+  <si>
+    <t>Maybe I should kill myself</t>
+  </si>
+  <si>
+    <t>Parking at 211 6th St. Las Vegas, NV 89101</t>
+  </si>
+  <si>
+    <t>Horchata</t>
   </si>
 </sst>
 </file>
@@ -1349,14 +1370,14 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1586,102 +1607,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1862,6 +1787,102 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2172,7 +2193,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>2/13/2026</a:t>
+            <a:t>2/19/2026</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -2319,7 +2340,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>2/13/2026</a:t>
+            <a:t>2/19/2026</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1">
             <a:solidFill>
@@ -2396,7 +2417,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>(0 days ago)</a:t>
+            <a:t>(1 days ago)</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1000" b="0">
             <a:solidFill>
@@ -2613,7 +2634,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>114</a:t>
+            <a:t>122</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
@@ -2686,7 +2707,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>(112 this year)</a:t>
+            <a:t>(120 this year)</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1050" b="1">
             <a:solidFill>
@@ -2907,7 +2928,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t> $2,878.17 </a:t>
+            <a:t> $2,513.36 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
@@ -3604,57 +3625,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28060ADD-D564-4882-ABCD-FDA2887A6DAF}" name="Income" displayName="Income" ref="C9:C14" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28060ADD-D564-4882-ABCD-FDA2887A6DAF}" name="Income" displayName="Income" ref="C9:C14" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="C9:C14" xr:uid="{28060ADD-D564-4882-ABCD-FDA2887A6DAF}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{19C7D09A-8E99-44B9-8A0D-52DA3AD6717B}" name="Income" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{19C7D09A-8E99-44B9-8A0D-52DA3AD6717B}" name="Income" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26EBFC05-007B-4DDB-99B1-923185513F43}" name="Expenses" displayName="Expenses" ref="C23:C41" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26EBFC05-007B-4DDB-99B1-923185513F43}" name="Expenses" displayName="Expenses" ref="C23:C41" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="C23:C41" xr:uid="{26EBFC05-007B-4DDB-99B1-923185513F43}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{054B0ED6-D229-4E7E-B46D-D8E9E2B6A652}" name="Expenses" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{054B0ED6-D229-4E7E-B46D-D8E9E2B6A652}" name="Expenses" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{732FC9EA-987F-4E96-95FB-D9D4C69B530B}" name="Savings" displayName="Savings" ref="C45:C52" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{732FC9EA-987F-4E96-95FB-D9D4C69B530B}" name="Savings" displayName="Savings" ref="C45:C52" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="C45:C52" xr:uid="{732FC9EA-987F-4E96-95FB-D9D4C69B530B}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9B015AA8-6AE7-4E7C-A9CB-340E9F2BCCE1}" name="Savings" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{9B015AA8-6AE7-4E7C-A9CB-340E9F2BCCE1}" name="Savings" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5EBDA7D6-5F78-4C14-BE92-7A3D34140449}" name="Tracking" displayName="Tracking" ref="B11:H222" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5EBDA7D6-5F78-4C14-BE92-7A3D34140449}" name="Tracking" displayName="Tracking" ref="B11:H222" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="B11:H222" xr:uid="{5EBDA7D6-5F78-4C14-BE92-7A3D34140449}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:H222">
     <sortCondition ref="B11:B222"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9596B93D-AE07-45FA-B9AB-1D752C5B70A5}" name="Date" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{053A61ED-D0C3-466D-9ADA-2118BEC6A477}" name="Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{36323927-3189-43D6-99B2-114D96B6071C}" name="Category" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{F50128DF-F86C-4CFD-A37C-5AF2310E1E1F}" name="Amount" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{F5BE8020-DEDC-4D8A-AE2A-D697C017C8F2}" name="Details" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{C39F81BF-FC60-4505-99E7-74D292B87A45}" name="Balance" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{9596B93D-AE07-45FA-B9AB-1D752C5B70A5}" name="Date" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{053A61ED-D0C3-466D-9ADA-2118BEC6A477}" name="Type" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{36323927-3189-43D6-99B2-114D96B6071C}" name="Category" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{F50128DF-F86C-4CFD-A37C-5AF2310E1E1F}" name="Amount" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{F5BE8020-DEDC-4D8A-AE2A-D697C017C8F2}" name="Details" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{C39F81BF-FC60-4505-99E7-74D292B87A45}" name="Balance" dataDxfId="27">
       <calculatedColumnFormula array="1">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B9EF5C2-38CE-4D67-86DA-7EBFDFFE3F50}" name="Effective Date" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{7B9EF5C2-38CE-4D67-86DA-7EBFDFFE3F50}" name="Effective Date" dataDxfId="26">
       <calculatedColumnFormula array="1">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4041,9 +4062,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="C5:CJ58"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B13" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B10" workbookViewId="0">
       <pane xSplit="3" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="T30" sqref="T30"/>
+      <selection pane="topRight" activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" outlineLevelCol="2" x14ac:dyDescent="0.25"/>
@@ -4072,102 +4093,102 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:88" x14ac:dyDescent="0.25">
-      <c r="E5" s="81" cm="1">
+      <c r="E5" s="83" cm="1">
         <f t="array" ref="E5">starting_year</f>
         <v>2025</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="S5" s="81">
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="S5" s="83">
         <f>E5+1</f>
         <v>2026</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="81"/>
-      <c r="Z5" s="81"/>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AG5" s="81">
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="83"/>
+      <c r="AD5" s="83"/>
+      <c r="AE5" s="83"/>
+      <c r="AG5" s="83">
         <f>S5+1</f>
         <v>2027</v>
       </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="81"/>
-      <c r="AN5" s="81"/>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AU5" s="81">
+      <c r="AH5" s="83"/>
+      <c r="AI5" s="83"/>
+      <c r="AJ5" s="83"/>
+      <c r="AK5" s="83"/>
+      <c r="AL5" s="83"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="83"/>
+      <c r="AO5" s="83"/>
+      <c r="AP5" s="83"/>
+      <c r="AQ5" s="83"/>
+      <c r="AR5" s="83"/>
+      <c r="AS5" s="83"/>
+      <c r="AU5" s="83">
         <f>AG5+1</f>
         <v>2028</v>
       </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="81"/>
-      <c r="BB5" s="81"/>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BI5" s="81">
+      <c r="AV5" s="83"/>
+      <c r="AW5" s="83"/>
+      <c r="AX5" s="83"/>
+      <c r="AY5" s="83"/>
+      <c r="AZ5" s="83"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="83"/>
+      <c r="BC5" s="83"/>
+      <c r="BD5" s="83"/>
+      <c r="BE5" s="83"/>
+      <c r="BF5" s="83"/>
+      <c r="BG5" s="83"/>
+      <c r="BI5" s="83">
         <f>AU5+1</f>
         <v>2029</v>
       </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="81"/>
-      <c r="BP5" s="81"/>
-      <c r="BQ5" s="81"/>
-      <c r="BR5" s="81"/>
-      <c r="BS5" s="81"/>
-      <c r="BT5" s="81"/>
-      <c r="BU5" s="81"/>
-      <c r="BW5" s="81">
+      <c r="BJ5" s="83"/>
+      <c r="BK5" s="83"/>
+      <c r="BL5" s="83"/>
+      <c r="BM5" s="83"/>
+      <c r="BN5" s="83"/>
+      <c r="BO5" s="83"/>
+      <c r="BP5" s="83"/>
+      <c r="BQ5" s="83"/>
+      <c r="BR5" s="83"/>
+      <c r="BS5" s="83"/>
+      <c r="BT5" s="83"/>
+      <c r="BU5" s="83"/>
+      <c r="BW5" s="83">
         <f>BI5+1</f>
         <v>2030</v>
       </c>
-      <c r="BX5" s="81"/>
-      <c r="BY5" s="81"/>
-      <c r="BZ5" s="81"/>
-      <c r="CA5" s="81"/>
-      <c r="CB5" s="81"/>
-      <c r="CC5" s="81"/>
-      <c r="CD5" s="81"/>
-      <c r="CE5" s="81"/>
-      <c r="CF5" s="81"/>
-      <c r="CG5" s="81"/>
-      <c r="CH5" s="81"/>
-      <c r="CI5" s="81"/>
+      <c r="BX5" s="83"/>
+      <c r="BY5" s="83"/>
+      <c r="BZ5" s="83"/>
+      <c r="CA5" s="83"/>
+      <c r="CB5" s="83"/>
+      <c r="CC5" s="83"/>
+      <c r="CD5" s="83"/>
+      <c r="CE5" s="83"/>
+      <c r="CF5" s="83"/>
+      <c r="CG5" s="83"/>
+      <c r="CH5" s="83"/>
+      <c r="CI5" s="83"/>
     </row>
     <row r="6" spans="3:88" x14ac:dyDescent="0.25">
       <c r="E6" s="19" t="str">
@@ -11654,8 +11675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83104009-D2B6-4A85-A17D-FEEFFDD93C2C}">
   <dimension ref="A1:J222"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A107" workbookViewId="0">
-      <selection activeCell="F125" sqref="F125"/>
+    <sheetView topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="D133" sqref="D133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11672,33 +11693,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -11707,19 +11728,19 @@
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="74">
         <f ca="1">Calculation!E8</f>
-        <v>46066</v>
+        <v>46072</v>
       </c>
       <c r="C8" s="74">
         <f>Calculation!E9</f>
-        <v>46066</v>
+        <v>46071</v>
       </c>
       <c r="D8" s="74" t="str">
         <f ca="1">Calculation!E10</f>
-        <v>(0 days ago)</v>
+        <v>(1 days ago)</v>
       </c>
       <c r="E8" s="75">
         <f>COUNT(Tracking[Date])</f>
-        <v>114</v>
+        <v>122</v>
       </c>
       <c r="F8" s="76"/>
       <c r="G8" s="77"/>
@@ -14548,123 +14569,203 @@
       </c>
     </row>
     <row r="126" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B126" s="37"/>
-      <c r="C126" s="38"/>
-      <c r="D126" s="38"/>
-      <c r="E126" s="39"/>
-      <c r="F126" s="38"/>
+      <c r="B126" s="37">
+        <v>46067</v>
+      </c>
+      <c r="C126" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D126" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E126" s="39">
+        <v>19.2</v>
+      </c>
+      <c r="F126" s="38" t="s">
+        <v>183</v>
+      </c>
       <c r="G126" s="40" cm="1">
         <f t="array" ref="G126">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2858.97</v>
       </c>
       <c r="H126" s="41" cm="1">
         <f t="array" ref="H126">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46067</v>
       </c>
     </row>
     <row r="127" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B127" s="37"/>
-      <c r="C127" s="38"/>
-      <c r="D127" s="38"/>
-      <c r="E127" s="39"/>
-      <c r="F127" s="38"/>
+      <c r="B127" s="37">
+        <v>46068</v>
+      </c>
+      <c r="C127" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D127" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E127" s="39">
+        <v>19.260000000000002</v>
+      </c>
+      <c r="F127" s="38" t="s">
+        <v>99</v>
+      </c>
       <c r="G127" s="40" cm="1">
         <f t="array" ref="G127">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2839.7099999999996</v>
       </c>
       <c r="H127" s="41" cm="1">
         <f t="array" ref="H127">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46068</v>
       </c>
     </row>
     <row r="128" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B128" s="37"/>
-      <c r="C128" s="38"/>
-      <c r="D128" s="38"/>
-      <c r="E128" s="39"/>
-      <c r="F128" s="38"/>
+      <c r="B128" s="37">
+        <v>46069</v>
+      </c>
+      <c r="C128" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D128" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E128" s="39">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="F128" s="38" t="s">
+        <v>184</v>
+      </c>
       <c r="G128" s="40" cm="1">
         <f t="array" ref="G128">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2820.22</v>
       </c>
       <c r="H128" s="41" cm="1">
         <f t="array" ref="H128">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46069</v>
       </c>
     </row>
     <row r="129" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B129" s="37"/>
-      <c r="C129" s="38"/>
-      <c r="D129" s="38"/>
-      <c r="E129" s="39"/>
-      <c r="F129" s="38"/>
+      <c r="B129" s="37">
+        <v>46070</v>
+      </c>
+      <c r="C129" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D129" s="38" t="s">
+        <v>22</v>
+      </c>
+      <c r="E129" s="39">
+        <v>14.08</v>
+      </c>
+      <c r="F129" s="38" t="s">
+        <v>185</v>
+      </c>
       <c r="G129" s="40" cm="1">
         <f t="array" ref="G129">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2532.2399999999998</v>
       </c>
       <c r="H129" s="41" cm="1">
         <f t="array" ref="H129">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46070</v>
       </c>
     </row>
     <row r="130" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B130" s="37"/>
-      <c r="C130" s="38"/>
-      <c r="D130" s="38"/>
-      <c r="E130" s="39"/>
-      <c r="F130" s="38"/>
+      <c r="B130" s="37">
+        <v>46070</v>
+      </c>
+      <c r="C130" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D130" s="38" t="s">
+        <v>20</v>
+      </c>
+      <c r="E130" s="39">
+        <v>123.9</v>
+      </c>
+      <c r="F130" s="38" t="s">
+        <v>186</v>
+      </c>
       <c r="G130" s="40" cm="1">
         <f t="array" ref="G130">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2532.2399999999998</v>
       </c>
       <c r="H130" s="41" cm="1">
         <f t="array" ref="H130">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46070</v>
       </c>
     </row>
     <row r="131" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B131" s="37"/>
-      <c r="C131" s="38"/>
-      <c r="D131" s="38"/>
-      <c r="E131" s="39"/>
-      <c r="F131" s="38"/>
+      <c r="B131" s="37">
+        <v>46070</v>
+      </c>
+      <c r="C131" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D131" s="38" t="s">
+        <v>125</v>
+      </c>
+      <c r="E131" s="39">
+        <v>150</v>
+      </c>
+      <c r="F131" s="38" t="s">
+        <v>187</v>
+      </c>
       <c r="G131" s="40" cm="1">
         <f t="array" ref="G131">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2532.2399999999998</v>
       </c>
       <c r="H131" s="41" cm="1">
         <f t="array" ref="H131">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46070</v>
       </c>
     </row>
     <row r="132" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B132" s="37"/>
-      <c r="C132" s="38"/>
-      <c r="D132" s="38"/>
-      <c r="E132" s="39"/>
-      <c r="F132" s="38"/>
+      <c r="B132" s="37">
+        <v>46071</v>
+      </c>
+      <c r="C132" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D132" s="38" t="s">
+        <v>124</v>
+      </c>
+      <c r="E132" s="39">
+        <v>5.99</v>
+      </c>
+      <c r="F132" s="38" t="s">
+        <v>188</v>
+      </c>
       <c r="G132" s="40" cm="1">
         <f t="array" ref="G132">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2513.36</v>
       </c>
       <c r="H132" s="41" cm="1">
         <f t="array" ref="H132">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="133" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B133" s="37"/>
-      <c r="C133" s="38"/>
-      <c r="D133" s="38"/>
-      <c r="E133" s="39"/>
-      <c r="F133" s="38"/>
+      <c r="B133" s="37">
+        <v>46071</v>
+      </c>
+      <c r="C133" s="38" t="s">
+        <v>7</v>
+      </c>
+      <c r="D133" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E133" s="39">
+        <v>12.89</v>
+      </c>
+      <c r="F133" s="38" t="s">
+        <v>189</v>
+      </c>
       <c r="G133" s="40" cm="1">
         <f t="array" ref="G133">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2513.36</v>
       </c>
       <c r="H133" s="41" cm="1">
         <f t="array" ref="H133">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
@@ -16050,8 +16151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA52A06-33F8-469B-A07A-85685272E998}">
   <dimension ref="A1:AR60"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="Y34" sqref="Y34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="Z23" sqref="Z23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16132,7 +16233,7 @@
       <c r="AO9" s="87"/>
       <c r="AP9" s="87"/>
       <c r="AQ9" s="89">
-        <v>36586</v>
+        <v>36557</v>
       </c>
       <c r="AR9" s="89"/>
     </row>
@@ -16161,7 +16262,7 @@
       <c r="X11" s="55"/>
       <c r="Y11" s="84" t="str" cm="1">
         <f t="array" aca="1" ref="Y11" ca="1">"Breakdown - " &amp; IF(selected_period="Total Year","Total Year",selected_period_display) &amp; " " &amp; selected_year</f>
-        <v>Breakdown - March 2026</v>
+        <v>Breakdown - February 2026</v>
       </c>
       <c r="Z11" s="84"/>
       <c r="AA11" s="84"/>
@@ -16436,13 +16537,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>5146.8899999999994</v>
       </c>
       <c r="L14" s="24" cm="1">
         <f t="array" aca="1" ref="L14" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>5210.41</v>
+        <v>5083.34</v>
       </c>
       <c r="M14" s="62" cm="1">
         <f t="array" ref="M14">IF(is_cat,
@@ -16504,23 +16605,23 @@
       </c>
       <c r="Z14" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>5146.8899999999994</v>
       </c>
       <c r="AA14" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>5210.41</v>
+        <v>5083.34</v>
       </c>
       <c r="AB14" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.0125016229486912</v>
       </c>
       <c r="AC14" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>5210.41</v>
+        <v>0</v>
       </c>
       <c r="AD14" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>63.549999999999272</v>
       </c>
       <c r="AH14" s="72"/>
     </row>
@@ -16605,7 +16706,7 @@
       </c>
       <c r="P15" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q15" s="24" t="str">
         <f t="shared" si="4"/>
@@ -16617,7 +16718,7 @@
       </c>
       <c r="S15" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="T15" s="24" t="str">
         <f t="shared" si="7"/>
@@ -16625,7 +16726,7 @@
       </c>
       <c r="U15" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V15" s="24" t="str">
         <f t="shared" si="9"/>
@@ -16633,19 +16734,19 @@
       </c>
       <c r="W15" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X15" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="Y15" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Side Hustle (Net)</v>
+        <v>Misc.</v>
       </c>
       <c r="Z15" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>1779.85</v>
       </c>
       <c r="AA15" s="70">
         <f t="shared" ca="1" si="14"/>
@@ -16661,7 +16762,7 @@
       </c>
       <c r="AD15" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1779.85</v>
       </c>
     </row>
     <row r="16" spans="1:44" x14ac:dyDescent="0.25">
@@ -16745,7 +16846,7 @@
       </c>
       <c r="P16" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q16" s="24" t="str">
         <f t="shared" si="4"/>
@@ -16757,7 +16858,7 @@
       </c>
       <c r="S16" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="T16" s="24" t="str">
         <f t="shared" si="7"/>
@@ -16765,7 +16866,7 @@
       </c>
       <c r="U16" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V16" s="24" t="str">
         <f t="shared" si="9"/>
@@ -16773,15 +16874,15 @@
       </c>
       <c r="W16" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X16" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y16" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v xml:space="preserve">Divedends </v>
+        <v>Side Hustle (Net)</v>
       </c>
       <c r="Z16" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -16885,7 +16986,7 @@
       </c>
       <c r="P17" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q17" s="24" t="str">
         <f t="shared" si="4"/>
@@ -16897,7 +16998,7 @@
       </c>
       <c r="S17" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="T17" s="24" t="str">
         <f t="shared" si="7"/>
@@ -16905,7 +17006,7 @@
       </c>
       <c r="U17" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V17" s="24" t="str">
         <f t="shared" si="9"/>
@@ -16913,15 +17014,15 @@
       </c>
       <c r="W17" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X17" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Y17" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Rollover</v>
+        <v xml:space="preserve">Divedends </v>
       </c>
       <c r="Z17" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -16997,7 +17098,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>1779.85</v>
       </c>
       <c r="L18" s="24" cm="1">
         <f t="array" aca="1" ref="L18" ca="1">IF(OR(is_header,is_empty),"",
@@ -17025,7 +17126,7 @@
       </c>
       <c r="P18" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q18" s="24" t="str">
         <f t="shared" si="4"/>
@@ -17037,7 +17138,7 @@
       </c>
       <c r="S18" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="T18" s="24" t="str">
         <f t="shared" si="7"/>
@@ -17053,15 +17154,15 @@
       </c>
       <c r="W18" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="X18" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="Y18" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Misc.</v>
+        <v>Rollover</v>
       </c>
       <c r="Z18" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -17137,13 +17238,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>6926.74</v>
       </c>
       <c r="L19" s="24" cm="1">
         <f t="array" aca="1" ref="L19" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>5210.41</v>
+        <v>5083.34</v>
       </c>
       <c r="M19" s="62" t="str" cm="1">
         <f t="array" ref="M19">IF(is_cat,
@@ -17205,23 +17306,23 @@
       </c>
       <c r="Z19" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>6926.74</v>
       </c>
       <c r="AA19" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>5210.41</v>
+        <v>5083.34</v>
       </c>
       <c r="AB19" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.3626355899861113</v>
       </c>
       <c r="AC19" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>5210.41</v>
+        <v>0</v>
       </c>
       <c r="AD19" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>1843.3999999999996</v>
       </c>
     </row>
     <row r="20" spans="3:30" x14ac:dyDescent="0.25">
@@ -17557,7 +17658,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>1280</v>
       </c>
       <c r="L22" s="24" cm="1">
         <f t="array" aca="1" ref="L22" ca="1">IF(OR(is_header,is_empty),"",
@@ -17625,7 +17726,7 @@
       </c>
       <c r="Z22" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>1280</v>
       </c>
       <c r="AA22" s="70">
         <f t="shared" ca="1" si="14"/>
@@ -17633,11 +17734,11 @@
       </c>
       <c r="AB22" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC22" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>1280</v>
+        <v>0</v>
       </c>
       <c r="AD22" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -17697,13 +17798,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>813.59</v>
       </c>
       <c r="L23" s="24" cm="1">
         <f t="array" aca="1" ref="L23" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>747.02</v>
+        <v>796</v>
       </c>
       <c r="M23" s="62" cm="1">
         <f t="array" ref="M23">IF(is_cat,
@@ -17725,7 +17826,7 @@
       </c>
       <c r="P23" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q23" s="24" t="str">
         <f t="shared" si="4"/>
@@ -17737,7 +17838,7 @@
       </c>
       <c r="S23" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>22</v>
       </c>
       <c r="T23" s="24" t="str">
         <f t="shared" si="7"/>
@@ -17765,23 +17866,23 @@
       </c>
       <c r="Z23" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>813.59</v>
       </c>
       <c r="AA23" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>747.02</v>
+        <v>796</v>
       </c>
       <c r="AB23" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.0220979899497489</v>
       </c>
       <c r="AC23" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>747.02</v>
+        <v>0</v>
       </c>
       <c r="AD23" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>17.590000000000032</v>
       </c>
     </row>
     <row r="24" spans="3:30" x14ac:dyDescent="0.25">
@@ -17837,7 +17938,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>117.25</v>
       </c>
       <c r="L24" s="24" cm="1">
         <f t="array" aca="1" ref="L24" ca="1">IF(OR(is_header,is_empty),"",
@@ -17865,7 +17966,7 @@
       </c>
       <c r="P24" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="Q24" s="24" t="str">
         <f t="shared" si="4"/>
@@ -17873,11 +17974,11 @@
       </c>
       <c r="R24" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S24" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>16</v>
+        <v>87</v>
       </c>
       <c r="T24" s="24" t="str">
         <f t="shared" si="7"/>
@@ -17885,7 +17986,7 @@
       </c>
       <c r="U24" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="V24" s="24" t="str">
         <f t="shared" si="9"/>
@@ -17893,35 +17994,35 @@
       </c>
       <c r="W24" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="X24" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Y24" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Car Insurance</v>
+        <v>Travel</v>
       </c>
       <c r="Z24" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>424.62</v>
       </c>
       <c r="AA24" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>404.4</v>
+        <v>300</v>
       </c>
       <c r="AB24" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.4154</v>
       </c>
       <c r="AC24" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>404.4</v>
+        <v>0</v>
       </c>
       <c r="AD24" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>124.62</v>
       </c>
     </row>
     <row r="25" spans="3:30" x14ac:dyDescent="0.25">
@@ -18005,7 +18106,7 @@
       </c>
       <c r="P25" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q25" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18013,11 +18114,11 @@
       </c>
       <c r="R25" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="S25" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>15</v>
+        <v>146</v>
       </c>
       <c r="T25" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18025,7 +18126,7 @@
       </c>
       <c r="U25" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="V25" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18033,35 +18134,35 @@
       </c>
       <c r="W25" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="X25" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="Y25" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v xml:space="preserve">Fun/Activities </v>
+        <v>Gifts</v>
       </c>
       <c r="Z25" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="AA25" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="AB25" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.25</v>
       </c>
       <c r="AC25" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>300</v>
+        <v>0</v>
       </c>
       <c r="AD25" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="3:30" x14ac:dyDescent="0.25">
@@ -18117,7 +18218,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>202.4</v>
       </c>
       <c r="L26" s="24" cm="1">
         <f t="array" aca="1" ref="L26" ca="1">IF(OR(is_header,is_empty),"",
@@ -18145,7 +18246,7 @@
       </c>
       <c r="P26" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="Q26" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18153,11 +18254,11 @@
       </c>
       <c r="R26" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="S26" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="T26" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18165,7 +18266,7 @@
       </c>
       <c r="U26" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="V26" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18173,31 +18274,31 @@
       </c>
       <c r="W26" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X26" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="Y26" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Car Payments</v>
+        <v>Car Insurance</v>
       </c>
       <c r="Z26" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>202.4</v>
       </c>
       <c r="AA26" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>250</v>
+        <v>404.4</v>
       </c>
       <c r="AB26" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.50049455984174085</v>
       </c>
       <c r="AC26" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>250</v>
+        <v>201.99999999999997</v>
       </c>
       <c r="AD26" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -18285,7 +18386,7 @@
       </c>
       <c r="P27" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q27" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18293,11 +18394,11 @@
       </c>
       <c r="R27" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="S27" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>19</v>
+        <v>1410</v>
       </c>
       <c r="T27" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18305,7 +18406,7 @@
       </c>
       <c r="U27" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="V27" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18313,31 +18414,31 @@
       </c>
       <c r="W27" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="X27" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="Y27" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Benifits</v>
+        <v xml:space="preserve">Fun/Activities </v>
       </c>
       <c r="Z27" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>123.9</v>
       </c>
       <c r="AA27" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>204.76</v>
+        <v>549.35</v>
       </c>
       <c r="AB27" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.22553927368708473</v>
       </c>
       <c r="AC27" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>204.76</v>
+        <v>425.45000000000005</v>
       </c>
       <c r="AD27" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -18425,7 +18526,7 @@
       </c>
       <c r="P28" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q28" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18433,11 +18534,11 @@
       </c>
       <c r="R28" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="S28" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>113</v>
+        <v>1418</v>
       </c>
       <c r="T28" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18445,7 +18546,7 @@
       </c>
       <c r="U28" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="V28" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18453,31 +18554,31 @@
       </c>
       <c r="W28" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="X28" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="Y28" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Utilities</v>
+        <v>Benifits</v>
       </c>
       <c r="Z28" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>117.25</v>
       </c>
       <c r="AA28" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>200</v>
+        <v>204.76</v>
       </c>
       <c r="AB28" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.57262160578237942</v>
       </c>
       <c r="AC28" s="70">
         <f ca="1">IF(is_empty,"",IF(is_header,"Remaining",IF(out_budget-out_tracked&gt;0,out_budget-out_tracked,0)))</f>
-        <v>200</v>
+        <v>87.509999999999991</v>
       </c>
       <c r="AD28" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -18537,13 +18638,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>93.18</v>
       </c>
       <c r="L29" s="24" cm="1">
         <f t="array" aca="1" ref="L29" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="M29" s="62" cm="1">
         <f t="array" ref="M29">IF(is_cat,
@@ -18565,7 +18666,7 @@
       </c>
       <c r="P29" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="Q29" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18573,11 +18674,11 @@
       </c>
       <c r="R29" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="S29" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>911</v>
       </c>
       <c r="T29" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18585,7 +18686,7 @@
       </c>
       <c r="U29" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="V29" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18593,11 +18694,11 @@
       </c>
       <c r="W29" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="X29" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="Y29" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -18605,7 +18706,7 @@
       </c>
       <c r="Z29" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>21.56</v>
       </c>
       <c r="AA29" s="70">
         <f t="shared" ca="1" si="14"/>
@@ -18613,11 +18714,11 @@
       </c>
       <c r="AB29" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.10779999999999999</v>
       </c>
       <c r="AC29" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>200</v>
+        <v>178.44</v>
       </c>
       <c r="AD29" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -18677,7 +18778,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>21.56</v>
       </c>
       <c r="L30" s="24" cm="1">
         <f t="array" aca="1" ref="L30" ca="1">IF(OR(is_header,is_empty),"",
@@ -18705,7 +18806,7 @@
       </c>
       <c r="P30" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="Q30" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18713,11 +18814,11 @@
       </c>
       <c r="R30" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="S30" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>17</v>
+        <v>128</v>
       </c>
       <c r="T30" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18725,7 +18826,7 @@
       </c>
       <c r="U30" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="V30" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18741,7 +18842,7 @@
       </c>
       <c r="Y30" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Car Warranty</v>
+        <v>Car Payments</v>
       </c>
       <c r="Z30" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -18749,7 +18850,7 @@
       </c>
       <c r="AA30" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>151.66999999999999</v>
+        <v>250</v>
       </c>
       <c r="AB30" s="69">
         <f t="shared" ca="1" si="15"/>
@@ -18757,7 +18858,7 @@
       </c>
       <c r="AC30" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>151.66999999999999</v>
+        <v>250</v>
       </c>
       <c r="AD30" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -18817,13 +18918,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>424.62</v>
       </c>
       <c r="L31" s="24" cm="1">
         <f t="array" aca="1" ref="L31" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>0</v>
+        <v>300</v>
       </c>
       <c r="M31" s="62" cm="1">
         <f t="array" ref="M31">IF(is_cat,
@@ -18845,7 +18946,7 @@
       </c>
       <c r="P31" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="Q31" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18853,11 +18954,11 @@
       </c>
       <c r="R31" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="S31" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>113</v>
+        <v>45</v>
       </c>
       <c r="T31" s="24" t="str">
         <f t="shared" si="7"/>
@@ -18865,7 +18966,7 @@
       </c>
       <c r="U31" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="V31" s="24" t="str">
         <f t="shared" si="9"/>
@@ -18873,11 +18974,11 @@
       </c>
       <c r="W31" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="X31" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="Y31" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
@@ -18885,7 +18986,7 @@
       </c>
       <c r="Z31" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>429.33</v>
       </c>
       <c r="AA31" s="70">
         <f t="shared" ca="1" si="14"/>
@@ -18893,15 +18994,15 @@
       </c>
       <c r="AB31" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>4.2932999999999995</v>
       </c>
       <c r="AC31" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="AD31" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>329.33</v>
       </c>
     </row>
     <row r="32" spans="3:30" x14ac:dyDescent="0.25">
@@ -18957,7 +19058,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>39.35</v>
       </c>
       <c r="L32" s="24" cm="1">
         <f t="array" aca="1" ref="L32" ca="1">IF(OR(is_header,is_empty),"",
@@ -18985,7 +19086,7 @@
       </c>
       <c r="P32" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="Q32" s="24" t="str">
         <f t="shared" si="4"/>
@@ -18993,11 +19094,11 @@
       </c>
       <c r="R32" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="S32" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>112</v>
+        <v>1113</v>
       </c>
       <c r="T32" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19005,7 +19106,7 @@
       </c>
       <c r="U32" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="V32" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19013,31 +19114,31 @@
       </c>
       <c r="W32" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="X32" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="Y32" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Media/Entertainment</v>
+        <v>Utilities</v>
       </c>
       <c r="Z32" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>93.18</v>
       </c>
       <c r="AA32" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>100</v>
+        <v>150</v>
       </c>
       <c r="AB32" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.62120000000000009</v>
       </c>
       <c r="AC32" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>100</v>
+        <v>56.819999999999993</v>
       </c>
       <c r="AD32" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -19103,7 +19204,7 @@
         <f t="array" aca="1" ref="L33" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="M33" s="62" cm="1">
         <f t="array" ref="M33">IF(is_cat,
@@ -19125,7 +19226,7 @@
       </c>
       <c r="P33" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q33" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19133,11 +19234,11 @@
       </c>
       <c r="R33" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="S33" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>113</v>
+        <v>1415</v>
       </c>
       <c r="T33" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19145,7 +19246,7 @@
       </c>
       <c r="U33" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="V33" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19153,31 +19254,31 @@
       </c>
       <c r="W33" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="X33" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="Y33" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Transportation</v>
+        <v>Media/Entertainment</v>
       </c>
       <c r="Z33" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>67.44</v>
       </c>
       <c r="AA33" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>80</v>
+        <v>70</v>
       </c>
       <c r="AB33" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.96342857142857141</v>
       </c>
       <c r="AC33" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>80</v>
+        <v>2.5600000000000023</v>
       </c>
       <c r="AD33" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -19237,7 +19338,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>429.33</v>
       </c>
       <c r="L34" s="24" cm="1">
         <f t="array" aca="1" ref="L34" ca="1">IF(OR(is_header,is_empty),"",
@@ -19265,7 +19366,7 @@
       </c>
       <c r="P34" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Q34" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19273,11 +19374,11 @@
       </c>
       <c r="R34" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="S34" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>110</v>
+        <v>312</v>
       </c>
       <c r="T34" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19301,23 +19402,23 @@
       </c>
       <c r="Y34" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Medical</v>
+        <v>Transportation</v>
       </c>
       <c r="Z34" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>39.35</v>
       </c>
       <c r="AA34" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AB34" s="69" t="str">
+        <v>80</v>
+      </c>
+      <c r="AB34" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>-</v>
+        <v>0.49187500000000001</v>
       </c>
       <c r="AC34" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>40.65</v>
       </c>
       <c r="AD34" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -19377,13 +19478,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>67.44</v>
       </c>
       <c r="L35" s="24" cm="1">
         <f t="array" aca="1" ref="L35" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>100</v>
+        <v>70</v>
       </c>
       <c r="M35" s="62" cm="1">
         <f t="array" ref="M35">IF(is_cat,
@@ -19405,7 +19506,7 @@
       </c>
       <c r="P35" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="Q35" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19413,11 +19514,11 @@
       </c>
       <c r="R35" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="S35" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>110</v>
+        <v>1014</v>
       </c>
       <c r="T35" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19425,7 +19526,7 @@
       </c>
       <c r="U35" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="V35" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19433,27 +19534,27 @@
       </c>
       <c r="W35" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X35" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="Y35" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Travel</v>
+        <v>Charity</v>
       </c>
       <c r="Z35" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>19.13</v>
       </c>
       <c r="AA35" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AB35" s="69" t="str">
+        <v>12.993</v>
+      </c>
+      <c r="AB35" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>-</v>
+        <v>1.4723312552913106</v>
       </c>
       <c r="AC35" s="70">
         <f t="shared" ca="1" si="16"/>
@@ -19461,7 +19562,7 @@
       </c>
       <c r="AD35" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>6.1369999999999987</v>
       </c>
     </row>
     <row r="36" spans="3:30" x14ac:dyDescent="0.25">
@@ -19517,13 +19618,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>123.9</v>
       </c>
       <c r="L36" s="24" cm="1">
         <f t="array" aca="1" ref="L36" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>300</v>
+        <v>549.35</v>
       </c>
       <c r="M36" s="62" cm="1">
         <f t="array" ref="M36">IF(is_cat,
@@ -19545,7 +19646,7 @@
       </c>
       <c r="P36" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="Q36" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19553,11 +19654,11 @@
       </c>
       <c r="R36" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="S36" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>73</v>
       </c>
       <c r="T36" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19565,7 +19666,7 @@
       </c>
       <c r="U36" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="V36" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19573,15 +19674,15 @@
       </c>
       <c r="W36" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="X36" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="Y36" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Clothing</v>
+        <v>Car Warranty</v>
       </c>
       <c r="Z36" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -19589,15 +19690,15 @@
       </c>
       <c r="AA36" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AB36" s="69" t="str">
+        <v>151.66999999999999</v>
+      </c>
+      <c r="AB36" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="AC36" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>151.66999999999999</v>
       </c>
       <c r="AD36" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -19663,7 +19764,7 @@
         <f t="array" aca="1" ref="L37" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="M37" s="62" cm="1">
         <f t="array" ref="M37">IF(is_cat,
@@ -19685,7 +19786,7 @@
       </c>
       <c r="P37" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="Q37" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19693,11 +19794,11 @@
       </c>
       <c r="R37" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="S37" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>113</v>
+        <v>1416</v>
       </c>
       <c r="T37" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19705,7 +19806,7 @@
       </c>
       <c r="U37" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="V37" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19713,15 +19814,15 @@
       </c>
       <c r="W37" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X37" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="Y37" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Body Care &amp; Medicine</v>
+        <v>Clothing</v>
       </c>
       <c r="Z37" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -19729,15 +19830,15 @@
       </c>
       <c r="AA37" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AB37" s="69" t="str">
+        <v>50</v>
+      </c>
+      <c r="AB37" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="AD37" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -19797,13 +19898,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>250</v>
       </c>
       <c r="L38" s="24" cm="1">
         <f t="array" aca="1" ref="L38" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>0</v>
+        <v>200</v>
       </c>
       <c r="M38" s="62" cm="1">
         <f t="array" ref="M38">IF(is_cat,
@@ -19825,7 +19926,7 @@
       </c>
       <c r="P38" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="Q38" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19833,11 +19934,11 @@
       </c>
       <c r="R38" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="S38" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>113</v>
+        <v>58</v>
       </c>
       <c r="T38" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19845,7 +19946,7 @@
       </c>
       <c r="U38" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="V38" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19853,15 +19954,15 @@
       </c>
       <c r="W38" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="X38" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="Y38" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Gifts</v>
+        <v>Body Care &amp; Medicine</v>
       </c>
       <c r="Z38" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -19869,15 +19970,15 @@
       </c>
       <c r="AA38" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="AB38" s="69" t="str">
+        <v>30</v>
+      </c>
+      <c r="AB38" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>-</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="AD38" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -19937,13 +20038,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>19.13</v>
       </c>
       <c r="L39" s="24" cm="1">
         <f t="array" aca="1" ref="L39" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>0</v>
+        <v>12.993</v>
       </c>
       <c r="M39" s="62" cm="1">
         <f t="array" ref="M39">IF(is_cat,
@@ -19965,7 +20066,7 @@
       </c>
       <c r="P39" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="Q39" s="24" t="str">
         <f t="shared" si="4"/>
@@ -19973,11 +20074,11 @@
       </c>
       <c r="R39" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="S39" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>113</v>
+        <v>1317</v>
       </c>
       <c r="T39" s="24" t="str">
         <f t="shared" si="7"/>
@@ -19985,7 +20086,7 @@
       </c>
       <c r="U39" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="V39" s="24" t="str">
         <f t="shared" si="9"/>
@@ -19993,15 +20094,15 @@
       </c>
       <c r="W39" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="X39" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="Y39" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Charity</v>
+        <v>Medical</v>
       </c>
       <c r="Z39" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -20077,13 +20178,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>3881.7499999999982</v>
       </c>
       <c r="L40" s="24" cm="1">
         <f t="array" aca="1" ref="L40" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>4017.85</v>
+        <v>4829.1730000000007</v>
       </c>
       <c r="M40" s="62" t="str" cm="1">
         <f t="array" ref="M40">IF(is_cat,
@@ -20145,19 +20246,19 @@
       </c>
       <c r="Z40" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>3881.7499999999982</v>
       </c>
       <c r="AA40" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>4017.85</v>
+        <v>4829.1730000000007</v>
       </c>
       <c r="AB40" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>0.80381257826132912</v>
       </c>
       <c r="AC40" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>4017.85</v>
+        <v>947.4230000000025</v>
       </c>
       <c r="AD40" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -20503,7 +20604,7 @@
         <f t="array" aca="1" ref="L43" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="M43" s="62" cm="1">
         <f t="array" ref="M43">IF(is_cat,
@@ -20525,7 +20626,7 @@
       </c>
       <c r="P43" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q43" s="24" t="str">
         <f t="shared" si="4"/>
@@ -20533,11 +20634,11 @@
       </c>
       <c r="R43" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S43" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="T43" s="24" t="str">
         <f t="shared" si="7"/>
@@ -20545,7 +20646,7 @@
       </c>
       <c r="U43" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V43" s="24" t="str">
         <f t="shared" si="9"/>
@@ -20553,35 +20654,35 @@
       </c>
       <c r="W43" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X43" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="Y43" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>Emergency Fund</v>
+        <v>401K</v>
       </c>
       <c r="Z43" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>257.33999999999997</v>
       </c>
       <c r="AA43" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>400</v>
+        <v>254.167</v>
       </c>
       <c r="AB43" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.0124839180538778</v>
       </c>
       <c r="AC43" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>400</v>
+        <v>0</v>
       </c>
       <c r="AD43" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>3.1729999999999734</v>
       </c>
     </row>
     <row r="44" spans="3:30" x14ac:dyDescent="0.25">
@@ -20637,13 +20738,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>257.33999999999997</v>
       </c>
       <c r="L44" s="24" cm="1">
         <f t="array" aca="1" ref="L44" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>254.17</v>
+        <v>254.167</v>
       </c>
       <c r="M44" s="62" cm="1">
         <f t="array" ref="M44">IF(is_cat,
@@ -20673,11 +20774,11 @@
       </c>
       <c r="R44" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="S44" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T44" s="24" t="str">
         <f t="shared" si="7"/>
@@ -20685,7 +20786,7 @@
       </c>
       <c r="U44" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="V44" s="24" t="str">
         <f t="shared" si="9"/>
@@ -20693,15 +20794,15 @@
       </c>
       <c r="W44" s="61">
         <f t="shared" ca="1" si="10"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="X44" s="67">
         <f t="shared" ca="1" si="11"/>
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="Y44" s="68" t="str">
         <f t="shared" ca="1" si="12"/>
-        <v>401K</v>
+        <v>Emergency Fund</v>
       </c>
       <c r="Z44" s="70">
         <f t="shared" ca="1" si="13"/>
@@ -20709,15 +20810,15 @@
       </c>
       <c r="AA44" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>254.17</v>
-      </c>
-      <c r="AB44" s="69">
+        <v>0</v>
+      </c>
+      <c r="AB44" s="69" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="AC44" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>254.17</v>
+        <v>0</v>
       </c>
       <c r="AD44" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -20783,7 +20884,7 @@
         <f t="array" aca="1" ref="L45" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="M45" s="62" cm="1">
         <f t="array" ref="M45">IF(is_cat,
@@ -20805,7 +20906,7 @@
       </c>
       <c r="P45" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q45" s="24" t="str">
         <f t="shared" si="4"/>
@@ -20813,11 +20914,11 @@
       </c>
       <c r="R45" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S45" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="T45" s="24" t="str">
         <f t="shared" si="7"/>
@@ -20825,7 +20926,7 @@
       </c>
       <c r="U45" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="V45" s="24" t="str">
         <f t="shared" si="9"/>
@@ -20849,15 +20950,15 @@
       </c>
       <c r="AA45" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>250</v>
-      </c>
-      <c r="AB45" s="69">
+        <v>0</v>
+      </c>
+      <c r="AB45" s="69" t="str">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>-</v>
       </c>
       <c r="AC45" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>250</v>
+        <v>0</v>
       </c>
       <c r="AD45" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -20945,7 +21046,7 @@
       </c>
       <c r="P46" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q46" s="24" t="str">
         <f t="shared" si="4"/>
@@ -20953,11 +21054,11 @@
       </c>
       <c r="R46" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S46" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T46" s="24" t="str">
         <f t="shared" si="7"/>
@@ -20965,7 +21066,7 @@
       </c>
       <c r="U46" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V46" s="24" t="str">
         <f t="shared" si="9"/>
@@ -21085,7 +21186,7 @@
       </c>
       <c r="P47" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q47" s="24" t="str">
         <f t="shared" si="4"/>
@@ -21093,11 +21194,11 @@
       </c>
       <c r="R47" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S47" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T47" s="24" t="str">
         <f t="shared" si="7"/>
@@ -21105,7 +21206,7 @@
       </c>
       <c r="U47" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V47" s="24" t="str">
         <f t="shared" si="9"/>
@@ -21225,7 +21326,7 @@
       </c>
       <c r="P48" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q48" s="24" t="str">
         <f t="shared" si="4"/>
@@ -21233,11 +21334,11 @@
       </c>
       <c r="R48" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S48" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T48" s="24" t="str">
         <f t="shared" si="7"/>
@@ -21245,7 +21346,7 @@
       </c>
       <c r="U48" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V48" s="24" t="str">
         <f t="shared" si="9"/>
@@ -21365,7 +21466,7 @@
       </c>
       <c r="P49" s="24">
         <f t="shared" ca="1" si="3"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Q49" s="24" t="str">
         <f t="shared" si="4"/>
@@ -21373,11 +21474,11 @@
       </c>
       <c r="R49" s="24">
         <f t="shared" ca="1" si="5"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="S49" s="62">
         <f t="shared" ca="1" si="6"/>
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="T49" s="24" t="str">
         <f t="shared" si="7"/>
@@ -21385,7 +21486,7 @@
       </c>
       <c r="U49" s="24">
         <f t="shared" ca="1" si="8"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="V49" s="24" t="str">
         <f t="shared" si="9"/>
@@ -21477,13 +21578,13 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>0</v>
+        <v>257.33999999999997</v>
       </c>
       <c r="L50" s="24" cm="1">
         <f t="array" aca="1" ref="L50" ca="1">IF(OR(is_header,is_empty),"",
 INDEX('Budget Planning'!$E:$CI,row_id,
 MATCH(IF(selected_period="Total Year",selected_year,DATE(selected_year,selected_period,1)),'Budget Planning'!$E$9:$CI$9,0)))</f>
-        <v>904.17</v>
+        <v>254.167</v>
       </c>
       <c r="M50" s="62" t="str" cm="1">
         <f t="array" ref="M50">IF(is_cat,
@@ -21545,23 +21646,23 @@
       </c>
       <c r="Z50" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>0</v>
+        <v>257.33999999999997</v>
       </c>
       <c r="AA50" s="70">
         <f t="shared" ca="1" si="14"/>
-        <v>904.17</v>
+        <v>254.167</v>
       </c>
       <c r="AB50" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0</v>
+        <v>1.0124839180538778</v>
       </c>
       <c r="AC50" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>904.17</v>
+        <v>0</v>
       </c>
       <c r="AD50" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>0</v>
+        <v>3.1729999999999734</v>
       </c>
     </row>
     <row r="51" spans="3:30" x14ac:dyDescent="0.25">
@@ -23255,7 +23356,7 @@
       </c>
       <c r="E8" s="36" cm="1">
         <f t="array" aca="1" ref="E8" ca="1">current_date</f>
-        <v>46066</v>
+        <v>46072</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.25">
@@ -23264,7 +23365,7 @@
       </c>
       <c r="E9" s="36">
         <f>MAX(Tracking[Date])</f>
-        <v>46066</v>
+        <v>46071</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.25">
@@ -23273,7 +23374,7 @@
       </c>
       <c r="E10" s="24" t="str">
         <f ca="1">IF(E9=0,"","(" &amp; _xlfn.DAYS(E8,E9) &amp; " days ago)")</f>
-        <v>(0 days ago)</v>
+        <v>(1 days ago)</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -23282,7 +23383,7 @@
       </c>
       <c r="E11" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">"(" &amp; SUMPRODUCT(--(YEAR(Tracking[Date])=YEAR(current_date))) &amp; " this year)"</f>
-        <v>(112 this year)</v>
+        <v>(120 this year)</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -23291,7 +23392,7 @@
       </c>
       <c r="E12" s="35">
         <f>INDEX(Tracking[Balance],MATCH(E9,Tracking[Date],0))</f>
-        <v>2878.1699999999996</v>
+        <v>2513.36</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -23353,7 +23454,7 @@
       </c>
       <c r="E21" s="24" cm="1">
         <f t="array" ref="E21">IF('Budget Dashboard'!AQ9="Total Year","Total Year",IF('Budget Dashboard'!AQ9="Current Month",MONTH(current_date),MONTH('Budget Dashboard'!AQ9)))</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="3:6" x14ac:dyDescent="0.25">
@@ -23362,7 +23463,7 @@
       </c>
       <c r="E22" s="53" t="str" cm="1">
         <f t="array" ref="E22">IF(selected_period="Total Year","Total Year",TEXT(DATE(2000,selected_period,1),"mmmm"))</f>
-        <v>March</v>
+        <v>February</v>
       </c>
     </row>
     <row r="23" spans="3:6" x14ac:dyDescent="0.25">
@@ -23404,14 +23505,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
@@ -23444,14 +23545,14 @@
       <c r="H7" s="30"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="23"/>

</xml_diff>

<commit_message>
Forgot I got Dutch Bros too
</commit_message>
<xml_diff>
--- a/Budget Plan.xlsx
+++ b/Budget Plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toolupcom-my.sharepoint.com/personal/solomon_manamel_pcstools_com/Documents/Desktop/P/Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://toolupcom-my.sharepoint.com/personal/solomon_manamel_pcstools_com/Documents/Desktop/Personal/Planning/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="149" documentId="13_ncr:1_{4B516CEF-07BC-46FE-AFFB-163B992373ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F327835F-6EEE-4147-9C5C-0EB3B30AE9D7}"/>
+  <xr:revisionPtr revIDLastSave="155" documentId="13_ncr:1_{4B516CEF-07BC-46FE-AFFB-163B992373ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{30FE4244-8CE6-49E8-AF80-BEA8E6F1A855}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="1770" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="191">
   <si>
     <t>To be allocated:</t>
   </si>
@@ -685,7 +685,7 @@
     <t>Horchata</t>
   </si>
   <si>
-    <t>test</t>
+    <t xml:space="preserve">Dutch Bro's </t>
   </si>
 </sst>
 </file>
@@ -1373,14 +1373,14 @@
         </ext>
       </extLst>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1610,102 +1610,6 @@
     </dxf>
     <dxf>
       <font>
-        <color theme="0" tint="-0.249977111117893"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.499984740745262"/>
-      </font>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="right" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="none">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="10"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="0"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" relativeIndent="1"/>
-    </dxf>
-    <dxf>
-      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1886,6 +1790,102 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.249977111117893"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.499984740745262"/>
+      </font>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="1" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="none">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="10"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" relativeIndent="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -2637,7 +2637,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>122</a:t>
+            <a:t>123</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
@@ -2710,7 +2710,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t>(120 this year)</a:t>
+            <a:t>(121 this year)</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1050" b="1">
             <a:solidFill>
@@ -2931,7 +2931,7 @@
               <a:latin typeface="Aptos Narrow"/>
             </a:rPr>
             <a:pPr/>
-            <a:t> $2,513.36 </a:t>
+            <a:t> $2,496.54 </a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
@@ -3628,57 +3628,57 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28060ADD-D564-4882-ABCD-FDA2887A6DAF}" name="Income" displayName="Income" ref="C9:C14" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{28060ADD-D564-4882-ABCD-FDA2887A6DAF}" name="Income" displayName="Income" ref="C9:C14" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="C9:C14" xr:uid="{28060ADD-D564-4882-ABCD-FDA2887A6DAF}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{19C7D09A-8E99-44B9-8A0D-52DA3AD6717B}" name="Income" dataDxfId="32"/>
+    <tableColumn id="1" xr3:uid="{19C7D09A-8E99-44B9-8A0D-52DA3AD6717B}" name="Income" dataDxfId="23"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26EBFC05-007B-4DDB-99B1-923185513F43}" name="Expenses" displayName="Expenses" ref="C23:C41" totalsRowShown="0" headerRowDxfId="31" dataDxfId="30">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{26EBFC05-007B-4DDB-99B1-923185513F43}" name="Expenses" displayName="Expenses" ref="C23:C41" totalsRowShown="0" headerRowDxfId="22" dataDxfId="21">
   <autoFilter ref="C23:C41" xr:uid="{26EBFC05-007B-4DDB-99B1-923185513F43}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{054B0ED6-D229-4E7E-B46D-D8E9E2B6A652}" name="Expenses" dataDxfId="29"/>
+    <tableColumn id="1" xr3:uid="{054B0ED6-D229-4E7E-B46D-D8E9E2B6A652}" name="Expenses" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{732FC9EA-987F-4E96-95FB-D9D4C69B530B}" name="Savings" displayName="Savings" ref="C45:C52" totalsRowShown="0" headerRowDxfId="28" dataDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{732FC9EA-987F-4E96-95FB-D9D4C69B530B}" name="Savings" displayName="Savings" ref="C45:C52" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
   <autoFilter ref="C45:C52" xr:uid="{732FC9EA-987F-4E96-95FB-D9D4C69B530B}">
     <filterColumn colId="0" hiddenButton="1"/>
   </autoFilter>
   <tableColumns count="1">
-    <tableColumn id="1" xr3:uid="{9B015AA8-6AE7-4E7C-A9CB-340E9F2BCCE1}" name="Savings" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{9B015AA8-6AE7-4E7C-A9CB-340E9F2BCCE1}" name="Savings" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5EBDA7D6-5F78-4C14-BE92-7A3D34140449}" name="Tracking" displayName="Tracking" ref="B11:H222" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5EBDA7D6-5F78-4C14-BE92-7A3D34140449}" name="Tracking" displayName="Tracking" ref="B11:H222" totalsRowShown="0" headerRowDxfId="34" dataDxfId="33">
   <autoFilter ref="B11:H222" xr:uid="{5EBDA7D6-5F78-4C14-BE92-7A3D34140449}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B12:H222">
     <sortCondition ref="B11:B222"/>
   </sortState>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{9596B93D-AE07-45FA-B9AB-1D752C5B70A5}" name="Date" dataDxfId="23"/>
-    <tableColumn id="2" xr3:uid="{053A61ED-D0C3-466D-9ADA-2118BEC6A477}" name="Type" dataDxfId="22"/>
-    <tableColumn id="3" xr3:uid="{36323927-3189-43D6-99B2-114D96B6071C}" name="Category" dataDxfId="21"/>
-    <tableColumn id="4" xr3:uid="{F50128DF-F86C-4CFD-A37C-5AF2310E1E1F}" name="Amount" dataDxfId="20"/>
-    <tableColumn id="5" xr3:uid="{F5BE8020-DEDC-4D8A-AE2A-D697C017C8F2}" name="Details" dataDxfId="19"/>
-    <tableColumn id="6" xr3:uid="{C39F81BF-FC60-4505-99E7-74D292B87A45}" name="Balance" dataDxfId="18">
+    <tableColumn id="1" xr3:uid="{9596B93D-AE07-45FA-B9AB-1D752C5B70A5}" name="Date" dataDxfId="32"/>
+    <tableColumn id="2" xr3:uid="{053A61ED-D0C3-466D-9ADA-2118BEC6A477}" name="Type" dataDxfId="31"/>
+    <tableColumn id="3" xr3:uid="{36323927-3189-43D6-99B2-114D96B6071C}" name="Category" dataDxfId="30"/>
+    <tableColumn id="4" xr3:uid="{F50128DF-F86C-4CFD-A37C-5AF2310E1E1F}" name="Amount" dataDxfId="29"/>
+    <tableColumn id="5" xr3:uid="{F5BE8020-DEDC-4D8A-AE2A-D697C017C8F2}" name="Details" dataDxfId="28"/>
+    <tableColumn id="6" xr3:uid="{C39F81BF-FC60-4505-99E7-74D292B87A45}" name="Balance" dataDxfId="27">
       <calculatedColumnFormula array="1">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{7B9EF5C2-38CE-4D67-86DA-7EBFDFFE3F50}" name="Effective Date" dataDxfId="17">
+    <tableColumn id="7" xr3:uid="{7B9EF5C2-38CE-4D67-86DA-7EBFDFFE3F50}" name="Effective Date" dataDxfId="26">
       <calculatedColumnFormula array="1">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -4096,102 +4096,102 @@
   </cols>
   <sheetData>
     <row r="5" spans="3:88" x14ac:dyDescent="0.25">
-      <c r="E5" s="81" cm="1">
+      <c r="E5" s="83" cm="1">
         <f t="array" ref="E5">starting_year</f>
         <v>2025</v>
       </c>
-      <c r="F5" s="81"/>
-      <c r="G5" s="81"/>
-      <c r="H5" s="81"/>
-      <c r="I5" s="81"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
-      <c r="N5" s="81"/>
-      <c r="O5" s="81"/>
-      <c r="P5" s="81"/>
-      <c r="Q5" s="81"/>
-      <c r="S5" s="81">
+      <c r="F5" s="83"/>
+      <c r="G5" s="83"/>
+      <c r="H5" s="83"/>
+      <c r="I5" s="83"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
+      <c r="N5" s="83"/>
+      <c r="O5" s="83"/>
+      <c r="P5" s="83"/>
+      <c r="Q5" s="83"/>
+      <c r="S5" s="83">
         <f>E5+1</f>
         <v>2026</v>
       </c>
-      <c r="T5" s="81"/>
-      <c r="U5" s="81"/>
-      <c r="V5" s="81"/>
-      <c r="W5" s="81"/>
-      <c r="X5" s="81"/>
-      <c r="Y5" s="81"/>
-      <c r="Z5" s="81"/>
-      <c r="AA5" s="81"/>
-      <c r="AB5" s="81"/>
-      <c r="AC5" s="81"/>
-      <c r="AD5" s="81"/>
-      <c r="AE5" s="81"/>
-      <c r="AG5" s="81">
+      <c r="T5" s="83"/>
+      <c r="U5" s="83"/>
+      <c r="V5" s="83"/>
+      <c r="W5" s="83"/>
+      <c r="X5" s="83"/>
+      <c r="Y5" s="83"/>
+      <c r="Z5" s="83"/>
+      <c r="AA5" s="83"/>
+      <c r="AB5" s="83"/>
+      <c r="AC5" s="83"/>
+      <c r="AD5" s="83"/>
+      <c r="AE5" s="83"/>
+      <c r="AG5" s="83">
         <f>S5+1</f>
         <v>2027</v>
       </c>
-      <c r="AH5" s="81"/>
-      <c r="AI5" s="81"/>
-      <c r="AJ5" s="81"/>
-      <c r="AK5" s="81"/>
-      <c r="AL5" s="81"/>
-      <c r="AM5" s="81"/>
-      <c r="AN5" s="81"/>
-      <c r="AO5" s="81"/>
-      <c r="AP5" s="81"/>
-      <c r="AQ5" s="81"/>
-      <c r="AR5" s="81"/>
-      <c r="AS5" s="81"/>
-      <c r="AU5" s="81">
+      <c r="AH5" s="83"/>
+      <c r="AI5" s="83"/>
+      <c r="AJ5" s="83"/>
+      <c r="AK5" s="83"/>
+      <c r="AL5" s="83"/>
+      <c r="AM5" s="83"/>
+      <c r="AN5" s="83"/>
+      <c r="AO5" s="83"/>
+      <c r="AP5" s="83"/>
+      <c r="AQ5" s="83"/>
+      <c r="AR5" s="83"/>
+      <c r="AS5" s="83"/>
+      <c r="AU5" s="83">
         <f>AG5+1</f>
         <v>2028</v>
       </c>
-      <c r="AV5" s="81"/>
-      <c r="AW5" s="81"/>
-      <c r="AX5" s="81"/>
-      <c r="AY5" s="81"/>
-      <c r="AZ5" s="81"/>
-      <c r="BA5" s="81"/>
-      <c r="BB5" s="81"/>
-      <c r="BC5" s="81"/>
-      <c r="BD5" s="81"/>
-      <c r="BE5" s="81"/>
-      <c r="BF5" s="81"/>
-      <c r="BG5" s="81"/>
-      <c r="BI5" s="81">
+      <c r="AV5" s="83"/>
+      <c r="AW5" s="83"/>
+      <c r="AX5" s="83"/>
+      <c r="AY5" s="83"/>
+      <c r="AZ5" s="83"/>
+      <c r="BA5" s="83"/>
+      <c r="BB5" s="83"/>
+      <c r="BC5" s="83"/>
+      <c r="BD5" s="83"/>
+      <c r="BE5" s="83"/>
+      <c r="BF5" s="83"/>
+      <c r="BG5" s="83"/>
+      <c r="BI5" s="83">
         <f>AU5+1</f>
         <v>2029</v>
       </c>
-      <c r="BJ5" s="81"/>
-      <c r="BK5" s="81"/>
-      <c r="BL5" s="81"/>
-      <c r="BM5" s="81"/>
-      <c r="BN5" s="81"/>
-      <c r="BO5" s="81"/>
-      <c r="BP5" s="81"/>
-      <c r="BQ5" s="81"/>
-      <c r="BR5" s="81"/>
-      <c r="BS5" s="81"/>
-      <c r="BT5" s="81"/>
-      <c r="BU5" s="81"/>
-      <c r="BW5" s="81">
+      <c r="BJ5" s="83"/>
+      <c r="BK5" s="83"/>
+      <c r="BL5" s="83"/>
+      <c r="BM5" s="83"/>
+      <c r="BN5" s="83"/>
+      <c r="BO5" s="83"/>
+      <c r="BP5" s="83"/>
+      <c r="BQ5" s="83"/>
+      <c r="BR5" s="83"/>
+      <c r="BS5" s="83"/>
+      <c r="BT5" s="83"/>
+      <c r="BU5" s="83"/>
+      <c r="BW5" s="83">
         <f>BI5+1</f>
         <v>2030</v>
       </c>
-      <c r="BX5" s="81"/>
-      <c r="BY5" s="81"/>
-      <c r="BZ5" s="81"/>
-      <c r="CA5" s="81"/>
-      <c r="CB5" s="81"/>
-      <c r="CC5" s="81"/>
-      <c r="CD5" s="81"/>
-      <c r="CE5" s="81"/>
-      <c r="CF5" s="81"/>
-      <c r="CG5" s="81"/>
-      <c r="CH5" s="81"/>
-      <c r="CI5" s="81"/>
+      <c r="BX5" s="83"/>
+      <c r="BY5" s="83"/>
+      <c r="BZ5" s="83"/>
+      <c r="CA5" s="83"/>
+      <c r="CB5" s="83"/>
+      <c r="CC5" s="83"/>
+      <c r="CD5" s="83"/>
+      <c r="CE5" s="83"/>
+      <c r="CF5" s="83"/>
+      <c r="CG5" s="83"/>
+      <c r="CH5" s="83"/>
+      <c r="CI5" s="83"/>
     </row>
     <row r="6" spans="3:88" x14ac:dyDescent="0.25">
       <c r="E6" s="19" t="str">
@@ -11679,7 +11679,7 @@
   <dimension ref="A1:J222"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="D135" sqref="D135"/>
+      <selection activeCell="G134" sqref="G134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11696,33 +11696,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="82" t="s">
+      <c r="A1" s="81" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="82"/>
-      <c r="C1" s="82"/>
-      <c r="D1" s="82"/>
-      <c r="E1" s="82"/>
+      <c r="B1" s="81"/>
+      <c r="C1" s="81"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
     </row>
     <row r="2" spans="1:9" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="82"/>
-      <c r="B2" s="82"/>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
+      <c r="A2" s="81"/>
+      <c r="B2" s="81"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="83" t="s">
+      <c r="C6" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="D6" s="83"/>
-      <c r="E6" s="83"/>
-      <c r="F6" s="83"/>
-      <c r="G6" s="83"/>
-      <c r="H6" s="83"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
       <c r="I6" s="36"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -11743,7 +11743,7 @@
       </c>
       <c r="E8" s="75">
         <f>COUNT(Tracking[Date])</f>
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="76"/>
       <c r="G8" s="77"/>
@@ -14664,7 +14664,7 @@
       </c>
       <c r="G129" s="40" cm="1">
         <f t="array" ref="G129">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>2532.2399999999998</v>
+        <v>2515.4199999999996</v>
       </c>
       <c r="H129" s="41" cm="1">
         <f t="array" ref="H129">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
@@ -14689,7 +14689,7 @@
       </c>
       <c r="G130" s="40" cm="1">
         <f t="array" ref="G130">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>2532.2399999999998</v>
+        <v>2515.4199999999996</v>
       </c>
       <c r="H130" s="41" cm="1">
         <f t="array" ref="H130">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
@@ -14714,7 +14714,7 @@
       </c>
       <c r="G131" s="40" cm="1">
         <f t="array" ref="G131">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>2532.2399999999998</v>
+        <v>2515.4199999999996</v>
       </c>
       <c r="H131" s="41" cm="1">
         <f t="array" ref="H131">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
@@ -14739,7 +14739,7 @@
       </c>
       <c r="G132" s="40" cm="1">
         <f t="array" ref="G132">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>2513.36</v>
+        <v>2496.54</v>
       </c>
       <c r="H132" s="41" cm="1">
         <f t="array" ref="H132">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
@@ -14764,7 +14764,7 @@
       </c>
       <c r="G133" s="40" cm="1">
         <f t="array" ref="G133">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>2513.36</v>
+        <v>2496.54</v>
       </c>
       <c r="H133" s="41" cm="1">
         <f t="array" ref="H133">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
@@ -14772,20 +14772,28 @@
       </c>
     </row>
     <row r="134" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B134" s="37"/>
-      <c r="C134" s="38"/>
+      <c r="B134" s="37">
+        <v>46070</v>
+      </c>
+      <c r="C134" s="38" t="s">
+        <v>7</v>
+      </c>
       <c r="D134" s="38" t="s">
+        <v>18</v>
+      </c>
+      <c r="E134" s="39">
+        <v>16.82</v>
+      </c>
+      <c r="F134" s="38" t="s">
         <v>190</v>
       </c>
-      <c r="E134" s="39"/>
-      <c r="F134" s="38"/>
       <c r="G134" s="40" cm="1">
         <f t="array" ref="G134">SUMPRODUCT(Tracking[Amount],--(Tracking[Date]&lt;=Tracking[[#This Row],[Date]]),(Tracking[Type]&lt;&gt;"Income")*(-1) + (Tracking[Type]="Income"))</f>
-        <v>0</v>
+        <v>2515.4199999999996</v>
       </c>
       <c r="H134" s="41" cm="1">
         <f t="array" ref="H134">IF(AND(Tracking[[#This Row],[Type]]="Income",shift_late_income_status="Active",DAY(Tracking[[#This Row],[Date]])&gt;=shift_late_income_starting_day),DATE(YEAR(Tracking[[#This Row],[Date]]),MONTH(Tracking[[#This Row],[Date]])+1,1),Tracking[[#This Row],[Date]])</f>
-        <v>0</v>
+        <v>46070</v>
       </c>
     </row>
     <row r="135" spans="2:8" x14ac:dyDescent="0.25">
@@ -18991,7 +18999,7 @@
       </c>
       <c r="Z31" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>429.33</v>
+        <v>446.15</v>
       </c>
       <c r="AA31" s="70">
         <f t="shared" ca="1" si="14"/>
@@ -18999,7 +19007,7 @@
       </c>
       <c r="AB31" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>4.2932999999999995</v>
+        <v>4.4615</v>
       </c>
       <c r="AC31" s="70">
         <f t="shared" ca="1" si="16"/>
@@ -19007,7 +19015,7 @@
       </c>
       <c r="AD31" s="70">
         <f t="shared" ca="1" si="17"/>
-        <v>329.33</v>
+        <v>346.15</v>
       </c>
     </row>
     <row r="32" spans="3:30" x14ac:dyDescent="0.25">
@@ -19343,7 +19351,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>429.33</v>
+        <v>446.15</v>
       </c>
       <c r="L34" s="24" cm="1">
         <f t="array" aca="1" ref="L34" ca="1">IF(OR(is_header,is_empty),"",
@@ -20183,7 +20191,7 @@
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year)),
 SUM(Tracking[Amount] * (Tracking[Type]=type) * (Tracking[Category]=item) * (YEAR(Tracking[Effective Date])=selected_year) * (MONTH(Tracking[Effective Date])=selected_period)))
 ))</f>
-        <v>3881.7499999999982</v>
+        <v>3898.5699999999983</v>
       </c>
       <c r="L40" s="24" cm="1">
         <f t="array" aca="1" ref="L40" ca="1">IF(OR(is_header,is_empty),"",
@@ -20251,7 +20259,7 @@
       </c>
       <c r="Z40" s="70">
         <f t="shared" ca="1" si="13"/>
-        <v>3881.7499999999982</v>
+        <v>3898.5699999999983</v>
       </c>
       <c r="AA40" s="70">
         <f t="shared" ca="1" si="14"/>
@@ -20259,11 +20267,11 @@
       </c>
       <c r="AB40" s="69">
         <f t="shared" ca="1" si="15"/>
-        <v>0.80381257826132912</v>
+        <v>0.80729557628190118</v>
       </c>
       <c r="AC40" s="70">
         <f t="shared" ca="1" si="16"/>
-        <v>947.4230000000025</v>
+        <v>930.60300000000234</v>
       </c>
       <c r="AD40" s="70">
         <f t="shared" ca="1" si="17"/>
@@ -23388,7 +23396,7 @@
       </c>
       <c r="E11" s="24" t="str" cm="1">
         <f t="array" aca="1" ref="E11" ca="1">"(" &amp; SUMPRODUCT(--(YEAR(Tracking[Date])=YEAR(current_date))) &amp; " this year)"</f>
-        <v>(120 this year)</v>
+        <v>(121 this year)</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.25">
@@ -23397,7 +23405,7 @@
       </c>
       <c r="E12" s="35">
         <f>INDEX(Tracking[Balance],MATCH(E9,Tracking[Date],0))</f>
-        <v>2513.36</v>
+        <v>2496.54</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.25">
@@ -23510,14 +23518,14 @@
   </cols>
   <sheetData>
     <row r="4" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C4" s="81" t="s">
+      <c r="C4" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="D4" s="81"/>
-      <c r="E4" s="81"/>
-      <c r="F4" s="81"/>
-      <c r="G4" s="81"/>
-      <c r="H4" s="81"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="83"/>
+      <c r="F4" s="83"/>
+      <c r="G4" s="83"/>
+      <c r="H4" s="83"/>
     </row>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C5" s="23"/>
@@ -23550,14 +23558,14 @@
       <c r="H7" s="30"/>
     </row>
     <row r="9" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C9" s="81" t="s">
+      <c r="C9" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="81"/>
-      <c r="E9" s="81"/>
-      <c r="F9" s="81"/>
-      <c r="G9" s="81"/>
-      <c r="H9" s="81"/>
+      <c r="D9" s="83"/>
+      <c r="E9" s="83"/>
+      <c r="F9" s="83"/>
+      <c r="G9" s="83"/>
+      <c r="H9" s="83"/>
     </row>
     <row r="10" spans="3:8" x14ac:dyDescent="0.25">
       <c r="C10" s="23"/>

</xml_diff>